<commit_message>
trying to prove instantiation without reqd slot
</commit_message>
<xml_diff>
--- a/schemasheets/multival_tabular_tests/generated/excel/multival_tabular_tests_generated.xlsx
+++ b/schemasheets/multival_tabular_tests/generated/excel/multival_tabular_tests_generated.xlsx
@@ -4,11 +4,17 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Person" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Person1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Database" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Organization" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Person" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Pet" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Database1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Organization1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Person1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Pet1" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,17 +431,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>first_name</t>
+          <t>person_set</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>last_name</t>
+          <t>pet_set</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>hobbies</t>
+          <t>org_set</t>
         </is>
       </c>
     </row>
@@ -445,6 +451,117 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>org_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>pet_names</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>first_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>last_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>hobbies</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pet_names</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"tennis,cooking,sewing,fishing"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"tennis,cooking,sewing,fishing"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>pet_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>species</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -461,6 +578,73 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>person_set</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>pet_set</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>org_set</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>org_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>pet_names</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>first_name</t>
         </is>
       </c>
@@ -472,6 +656,42 @@
       <c r="C1" t="inlineStr">
         <is>
           <t>hobbies</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pet_names</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>pet_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>species</t>
         </is>
       </c>
     </row>

</xml_diff>